<commit_message>
Counts instead of binary features
</commit_message>
<xml_diff>
--- a/custom_model/initial_results.xlsx
+++ b/custom_model/initial_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="6375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
   <si>
     <t>Folds: 4</t>
   </si>
@@ -248,9 +248,6 @@
     <t>RESULTS WITH MIN_OCCURRANCES 4, SCORE &gt;50</t>
   </si>
   <si>
-    <t>WITH THE SUBSET OF FEATURES (OCCURS 40:100 times)</t>
-  </si>
-  <si>
     <t>Accuracy   0.736842  0.789474  0.684211</t>
   </si>
   <si>
@@ -306,6 +303,66 @@
   </si>
   <si>
     <t>F1         0.444444  0.484848  0.352941</t>
+  </si>
+  <si>
+    <t>WITH THE SUBSET OF FEATURES (OCCURS 40:100 times), note avg length didn't add anything</t>
+  </si>
+  <si>
+    <t>WITH SUBSET AND WORD COUNTS</t>
+  </si>
+  <si>
+    <t>Accuracy   0.789474  0.815789  0.684211</t>
+  </si>
+  <si>
+    <t>Precision  0.783784  0.823529  0.793103</t>
+  </si>
+  <si>
+    <t>F1         0.878788  0.888889  0.793103</t>
+  </si>
+  <si>
+    <t>Accuracy   0.368421  0.605263  0.631579</t>
+  </si>
+  <si>
+    <t>Precision  0.461538   0.62963  0.681818</t>
+  </si>
+  <si>
+    <t>Recall     0.545455  0.772727  0.681818</t>
+  </si>
+  <si>
+    <t>F1              0.5  0.693878  0.681818</t>
+  </si>
+  <si>
+    <t>Accuracy        0.5  0.578947  0.631579</t>
+  </si>
+  <si>
+    <t>Precision       0.5  0.545455       0.6</t>
+  </si>
+  <si>
+    <t>Recall     0.631579  0.947368  0.789474</t>
+  </si>
+  <si>
+    <t>F1          0.55814  0.692308  0.681818</t>
+  </si>
+  <si>
+    <t>Accuracy   0.763158  0.815789  0.710526</t>
+  </si>
+  <si>
+    <t>Precision  0.763158  0.823529  0.821429</t>
+  </si>
+  <si>
+    <t>F1         0.865672  0.888889  0.807018</t>
+  </si>
+  <si>
+    <t>Accuracy   0.631579  0.605263  0.421053</t>
+  </si>
+  <si>
+    <t>Precision  0.631579  0.642857       0.4</t>
+  </si>
+  <si>
+    <t>Recall     0.631579  0.473684  0.315789</t>
+  </si>
+  <si>
+    <t>F1         0.631579  0.545455  0.352941</t>
   </si>
 </sst>
 </file>
@@ -671,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,152 +1197,238 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>74</v>
+        <v>93</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="H70" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
+      <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H72" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
+      <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H78" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
+      <c r="H81" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
+      <c r="H82" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
+      <c r="H85" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
+      <c r="H86" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
+      <c r="H87" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H88" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H90" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H91" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
+      <c r="H93" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
+      <c r="H94" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+      <c r="H95" s="1"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
+      <c r="H97" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
+      <c r="H98" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
+      <c r="H99" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>93</v>
+      <c r="H100" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>